<commit_message>
Corrected to RK teams excels
</commit_message>
<xml_diff>
--- a/CompLaagRayon/files/template-excel-rk-25m1pijl-teams.xlsx
+++ b/CompLaagRayon/files/template-excel-rk-25m1pijl-teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\RK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCE889A-C3ED-40D4-BB5F-FC573DEB12B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF380102-5A93-4BD4-97D6-7E6C7CFB00BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="22440" windowHeight="14040" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="22440" windowHeight="14040" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="16" r:id="rId1"/>
@@ -1265,7 +1265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1512,12 +1512,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2179,10 +2173,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="135" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="137"/>
+      <c r="B4" s="135"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -2357,17 +2351,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="138" t="str">
+      <c r="B1" s="136" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>RK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="140"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="138"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C2" s="10"/>
@@ -2513,9 +2507,9 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.109375" style="64" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" style="116" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="116" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="116" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" style="114" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="114" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="114" customWidth="1"/>
     <col min="5" max="5" width="7.77734375" style="64" customWidth="1"/>
     <col min="6" max="6" width="34.44140625" style="64" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="65" customWidth="1"/>
@@ -2528,18 +2522,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="143"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="141"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="62"/>
@@ -2548,33 +2542,33 @@
       <c r="K3" s="67"/>
     </row>
     <row r="4" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="145" t="s">
+      <c r="B4" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="144"/>
       <c r="E4" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="147" t="s">
+      <c r="F4" s="145" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="148" t="s">
+      <c r="H4" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="149"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="147"/>
     </row>
     <row r="5" spans="2:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
       <c r="D5" s="72"/>
       <c r="E5" s="71"/>
-      <c r="F5" s="147"/>
+      <c r="F5" s="145"/>
       <c r="G5" s="71"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
@@ -2592,10 +2586,10 @@
       <c r="G6" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="144" t="s">
+      <c r="H6" s="142" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="144"/>
+      <c r="I6" s="142"/>
       <c r="J6" s="75" t="s">
         <v>1</v>
       </c>
@@ -2636,44 +2630,44 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="115"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="118"/>
+      <c r="B8" s="113"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="115"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="114"/>
+      <c r="K8" s="116"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="119">
+      <c r="B9" s="117">
         <v>1</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="118">
         <v>100</v>
       </c>
-      <c r="D9" s="121" t="s">
+      <c r="D9" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="121" t="s">
+      <c r="E9" s="118"/>
+      <c r="F9" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="122">
+      <c r="G9" s="120">
         <v>888.8</v>
       </c>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="123">
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="121">
         <f>IF(COUNTA(J10:J13)&lt;3,0,IF(COUNTA(J10:J13)=3,SUM(J10:J13),IF(SUM(J10:J13)&gt;0,SUM(J10:J13)-MINA(J10:J13),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="119"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
+      <c r="B10" s="117"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
       <c r="E10" s="8">
         <v>123456</v>
       </c>
@@ -2696,9 +2690,9 @@
       <c r="K10" s="67"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="119"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
       <c r="E11" s="8">
         <v>123456</v>
       </c>
@@ -2721,9 +2715,9 @@
       <c r="K11" s="67"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="119"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
       <c r="E12" s="8">
         <v>123456</v>
       </c>
@@ -2746,9 +2740,9 @@
       <c r="K12" s="67"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="119"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
       <c r="E13" s="8">
         <v>123456</v>
       </c>
@@ -2771,45 +2765,45 @@
       <c r="K13" s="67"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="119"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="129"/>
-      <c r="G14" s="130"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="123"/>
       <c r="K14" s="67"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="119">
+      <c r="B15" s="117">
         <v>2</v>
       </c>
-      <c r="C15" s="120">
+      <c r="C15" s="118">
         <v>100</v>
       </c>
-      <c r="D15" s="121" t="s">
+      <c r="D15" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="120"/>
-      <c r="F15" s="121" t="s">
+      <c r="E15" s="118"/>
+      <c r="F15" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="122">
+      <c r="G15" s="120">
         <v>888.8</v>
       </c>
-      <c r="H15" s="125"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="123">
+      <c r="H15" s="123"/>
+      <c r="I15" s="123"/>
+      <c r="J15" s="114"/>
+      <c r="K15" s="121">
         <f>IF(COUNTA(J16:J19)&lt;3,0,IF(COUNTA(J16:J19)=3,SUM(J16:J19),IF(SUM(J16:J19)&gt;0,SUM(J16:J19)-MINA(J16:J19),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="119"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
       <c r="E16" s="8">
         <v>123456</v>
       </c>
@@ -2832,9 +2826,9 @@
       <c r="K16" s="67"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="119"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="118"/>
       <c r="E17" s="8">
         <v>123456</v>
       </c>
@@ -2857,9 +2851,9 @@
       <c r="K17" s="67"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="119"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
       <c r="E18" s="8">
         <v>123456</v>
       </c>
@@ -2882,9 +2876,9 @@
       <c r="K18" s="67"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="119"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
       <c r="E19" s="8">
         <v>123456</v>
       </c>
@@ -2907,45 +2901,45 @@
       <c r="K19" s="67"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="119"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="125"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="123"/>
+      <c r="I20" s="123"/>
       <c r="K20" s="67"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="119">
+      <c r="B21" s="117">
         <v>3</v>
       </c>
-      <c r="C21" s="120">
+      <c r="C21" s="118">
         <v>100</v>
       </c>
-      <c r="D21" s="121" t="s">
+      <c r="D21" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="121" t="s">
+      <c r="E21" s="118"/>
+      <c r="F21" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="122">
+      <c r="G21" s="120">
         <v>888.8</v>
       </c>
-      <c r="H21" s="125"/>
-      <c r="I21" s="125"/>
-      <c r="J21" s="116"/>
-      <c r="K21" s="123">
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
+      <c r="J21" s="114"/>
+      <c r="K21" s="121">
         <f>IF(COUNTA(J22:J25)&lt;3,0,IF(COUNTA(J22:J25)=3,SUM(J22:J25),IF(SUM(J22:J25)&gt;0,SUM(J22:J25)-MINA(J22:J25),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="119"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
       <c r="E22" s="8">
         <v>123456</v>
       </c>
@@ -2968,9 +2962,9 @@
       <c r="K22" s="67"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="119"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
       <c r="E23" s="8">
         <v>123456</v>
       </c>
@@ -2993,9 +2987,9 @@
       <c r="K23" s="67"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="119"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="118"/>
       <c r="E24" s="8">
         <v>123456</v>
       </c>
@@ -3018,9 +3012,9 @@
       <c r="K24" s="67"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="119"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
       <c r="E25" s="8">
         <v>123456</v>
       </c>
@@ -3043,45 +3037,45 @@
       <c r="K25" s="67"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="119"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="129"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="125"/>
-      <c r="I26" s="125"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="127"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="123"/>
+      <c r="I26" s="123"/>
       <c r="K26" s="67"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="119">
+      <c r="B27" s="117">
         <v>4</v>
       </c>
-      <c r="C27" s="120">
+      <c r="C27" s="118">
         <v>100</v>
       </c>
-      <c r="D27" s="121" t="s">
+      <c r="D27" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="120"/>
-      <c r="F27" s="121" t="s">
+      <c r="E27" s="118"/>
+      <c r="F27" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="122">
+      <c r="G27" s="120">
         <v>888.8</v>
       </c>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="116"/>
-      <c r="K27" s="123">
+      <c r="H27" s="123"/>
+      <c r="I27" s="123"/>
+      <c r="J27" s="114"/>
+      <c r="K27" s="121">
         <f>IF(COUNTA(J28:J31)&lt;3,0,IF(COUNTA(J28:J31)=3,SUM(J28:J31),IF(SUM(J28:J31)&gt;0,SUM(J28:J31)-MINA(J28:J31),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="119"/>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="118"/>
       <c r="E28" s="8">
         <v>123456</v>
       </c>
@@ -3104,9 +3098,9 @@
       <c r="K28" s="67"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="119"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="120"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="118"/>
       <c r="E29" s="8">
         <v>123456</v>
       </c>
@@ -3129,9 +3123,9 @@
       <c r="K29" s="67"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="119"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
+      <c r="B30" s="117"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="118"/>
       <c r="E30" s="8">
         <v>123456</v>
       </c>
@@ -3154,9 +3148,9 @@
       <c r="K30" s="67"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="119"/>
-      <c r="C31" s="120"/>
-      <c r="D31" s="120"/>
+      <c r="B31" s="117"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="118"/>
       <c r="E31" s="8">
         <v>123456</v>
       </c>
@@ -3179,45 +3173,45 @@
       <c r="K31" s="67"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="119"/>
-      <c r="C32" s="120"/>
-      <c r="D32" s="120"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="129"/>
-      <c r="G32" s="130"/>
-      <c r="H32" s="125"/>
-      <c r="I32" s="125"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="127"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
       <c r="K32" s="67"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="119">
+      <c r="B33" s="117">
         <v>5</v>
       </c>
-      <c r="C33" s="120">
+      <c r="C33" s="118">
         <v>100</v>
       </c>
-      <c r="D33" s="121" t="s">
+      <c r="D33" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="120"/>
-      <c r="F33" s="121" t="s">
+      <c r="E33" s="118"/>
+      <c r="F33" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="122">
+      <c r="G33" s="120">
         <v>888.8</v>
       </c>
-      <c r="H33" s="125"/>
-      <c r="I33" s="125"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="123">
+      <c r="H33" s="123"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="114"/>
+      <c r="K33" s="121">
         <f>IF(COUNTA(J34:J37)&lt;3,0,IF(COUNTA(J34:J37)=3,SUM(J34:J37),IF(SUM(J34:J37)&gt;0,SUM(J34:J37)-MINA(J34:J37),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="119"/>
-      <c r="C34" s="120"/>
-      <c r="D34" s="120"/>
+      <c r="B34" s="117"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
       <c r="E34" s="8">
         <v>123456</v>
       </c>
@@ -3240,9 +3234,9 @@
       <c r="K34" s="67"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="119"/>
-      <c r="C35" s="120"/>
-      <c r="D35" s="120"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
       <c r="E35" s="8">
         <v>123456</v>
       </c>
@@ -3265,9 +3259,9 @@
       <c r="K35" s="67"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="119"/>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
+      <c r="B36" s="117"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="118"/>
       <c r="E36" s="8">
         <v>123456</v>
       </c>
@@ -3290,9 +3284,9 @@
       <c r="K36" s="67"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="119"/>
-      <c r="C37" s="120"/>
-      <c r="D37" s="120"/>
+      <c r="B37" s="117"/>
+      <c r="C37" s="118"/>
+      <c r="D37" s="118"/>
       <c r="E37" s="8">
         <v>123456</v>
       </c>
@@ -3315,45 +3309,45 @@
       <c r="K37" s="67"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="119"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="125"/>
-      <c r="F38" s="129"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="125"/>
-      <c r="I38" s="125"/>
+      <c r="B38" s="117"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="118"/>
+      <c r="E38" s="123"/>
+      <c r="F38" s="127"/>
+      <c r="G38" s="128"/>
+      <c r="H38" s="123"/>
+      <c r="I38" s="123"/>
       <c r="K38" s="67"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="119">
+      <c r="B39" s="117">
         <v>6</v>
       </c>
-      <c r="C39" s="120">
+      <c r="C39" s="118">
         <v>100</v>
       </c>
-      <c r="D39" s="121" t="s">
+      <c r="D39" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="120"/>
-      <c r="F39" s="121" t="s">
+      <c r="E39" s="118"/>
+      <c r="F39" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="122">
+      <c r="G39" s="120">
         <v>888.8</v>
       </c>
-      <c r="H39" s="125"/>
-      <c r="I39" s="125"/>
-      <c r="J39" s="116"/>
-      <c r="K39" s="123">
+      <c r="H39" s="123"/>
+      <c r="I39" s="123"/>
+      <c r="J39" s="114"/>
+      <c r="K39" s="121">
         <f>IF(COUNTA(J40:J43)&lt;3,0,IF(COUNTA(J40:J43)=3,SUM(J40:J43),IF(SUM(J40:J43)&gt;0,SUM(J40:J43)-MINA(J40:J43),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="119"/>
-      <c r="C40" s="120"/>
-      <c r="D40" s="120"/>
+      <c r="B40" s="117"/>
+      <c r="C40" s="118"/>
+      <c r="D40" s="118"/>
       <c r="E40" s="8">
         <v>123456</v>
       </c>
@@ -3376,9 +3370,9 @@
       <c r="K40" s="67"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="119"/>
-      <c r="C41" s="120"/>
-      <c r="D41" s="120"/>
+      <c r="B41" s="117"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="118"/>
       <c r="E41" s="8">
         <v>123456</v>
       </c>
@@ -3401,9 +3395,9 @@
       <c r="K41" s="67"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="119"/>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
+      <c r="B42" s="117"/>
+      <c r="C42" s="118"/>
+      <c r="D42" s="118"/>
       <c r="E42" s="8">
         <v>123456</v>
       </c>
@@ -3426,9 +3420,9 @@
       <c r="K42" s="67"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="119"/>
-      <c r="C43" s="120"/>
-      <c r="D43" s="120"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="118"/>
+      <c r="D43" s="118"/>
       <c r="E43" s="8">
         <v>123456</v>
       </c>
@@ -3451,45 +3445,45 @@
       <c r="K43" s="67"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="119"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="125"/>
-      <c r="I44" s="125"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="127"/>
+      <c r="G44" s="128"/>
+      <c r="H44" s="123"/>
+      <c r="I44" s="123"/>
       <c r="K44" s="67"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="119">
+      <c r="B45" s="117">
         <v>7</v>
       </c>
-      <c r="C45" s="120">
+      <c r="C45" s="118">
         <v>100</v>
       </c>
-      <c r="D45" s="121" t="s">
+      <c r="D45" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="120"/>
-      <c r="F45" s="121" t="s">
+      <c r="E45" s="118"/>
+      <c r="F45" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="122">
+      <c r="G45" s="120">
         <v>888.8</v>
       </c>
-      <c r="H45" s="125"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="116"/>
-      <c r="K45" s="123">
+      <c r="H45" s="123"/>
+      <c r="I45" s="123"/>
+      <c r="J45" s="114"/>
+      <c r="K45" s="121">
         <f>IF(COUNTA(J46:J49)&lt;3,0,IF(COUNTA(J46:J49)=3,SUM(J46:J49),IF(SUM(J46:J49)&gt;0,SUM(J46:J49)-MINA(J46:J49),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
-      <c r="D46" s="120"/>
+      <c r="B46" s="117"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
       <c r="E46" s="8">
         <v>123456</v>
       </c>
@@ -3512,9 +3506,9 @@
       <c r="K46" s="67"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="119"/>
-      <c r="C47" s="120"/>
-      <c r="D47" s="120"/>
+      <c r="B47" s="117"/>
+      <c r="C47" s="118"/>
+      <c r="D47" s="118"/>
       <c r="E47" s="8">
         <v>123456</v>
       </c>
@@ -3537,9 +3531,9 @@
       <c r="K47" s="67"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="119"/>
-      <c r="C48" s="120"/>
-      <c r="D48" s="120"/>
+      <c r="B48" s="117"/>
+      <c r="C48" s="118"/>
+      <c r="D48" s="118"/>
       <c r="E48" s="8">
         <v>123456</v>
       </c>
@@ -3562,9 +3556,9 @@
       <c r="K48" s="67"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="119"/>
-      <c r="C49" s="120"/>
-      <c r="D49" s="120"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="118"/>
       <c r="E49" s="8">
         <v>123456</v>
       </c>
@@ -3587,45 +3581,45 @@
       <c r="K49" s="67"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="119"/>
-      <c r="C50" s="120"/>
-      <c r="D50" s="120"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="129"/>
-      <c r="G50" s="130"/>
-      <c r="H50" s="125"/>
-      <c r="I50" s="125"/>
+      <c r="B50" s="117"/>
+      <c r="C50" s="118"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="123"/>
+      <c r="F50" s="127"/>
+      <c r="G50" s="128"/>
+      <c r="H50" s="123"/>
+      <c r="I50" s="123"/>
       <c r="K50" s="67"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="119">
+      <c r="B51" s="117">
         <v>8</v>
       </c>
-      <c r="C51" s="120">
+      <c r="C51" s="118">
         <v>100</v>
       </c>
-      <c r="D51" s="121" t="s">
+      <c r="D51" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="120"/>
-      <c r="F51" s="121" t="s">
+      <c r="E51" s="118"/>
+      <c r="F51" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="G51" s="122">
+      <c r="G51" s="120">
         <v>888.8</v>
       </c>
-      <c r="H51" s="125"/>
-      <c r="I51" s="125"/>
-      <c r="J51" s="116"/>
-      <c r="K51" s="123">
+      <c r="H51" s="123"/>
+      <c r="I51" s="123"/>
+      <c r="J51" s="114"/>
+      <c r="K51" s="121">
         <f>IF(COUNTA(J52:J55)&lt;3,0,IF(COUNTA(J52:J55)=3,SUM(J52:J55),IF(SUM(J52:J55)&gt;0,SUM(J52:J55)-MINA(J52:J55),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="119"/>
-      <c r="C52" s="120"/>
-      <c r="D52" s="120"/>
+      <c r="B52" s="117"/>
+      <c r="C52" s="118"/>
+      <c r="D52" s="118"/>
       <c r="E52" s="8">
         <v>123456</v>
       </c>
@@ -3648,9 +3642,9 @@
       <c r="K52" s="67"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B53" s="119"/>
-      <c r="C53" s="120"/>
-      <c r="D53" s="120"/>
+      <c r="B53" s="117"/>
+      <c r="C53" s="118"/>
+      <c r="D53" s="118"/>
       <c r="E53" s="8">
         <v>123456</v>
       </c>
@@ -3673,9 +3667,9 @@
       <c r="K53" s="67"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="119"/>
-      <c r="C54" s="120"/>
-      <c r="D54" s="120"/>
+      <c r="B54" s="117"/>
+      <c r="C54" s="118"/>
+      <c r="D54" s="118"/>
       <c r="E54" s="8">
         <v>123456</v>
       </c>
@@ -3698,9 +3692,9 @@
       <c r="K54" s="67"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B55" s="119"/>
-      <c r="C55" s="120"/>
-      <c r="D55" s="120"/>
+      <c r="B55" s="117"/>
+      <c r="C55" s="118"/>
+      <c r="D55" s="118"/>
       <c r="E55" s="8">
         <v>123456</v>
       </c>
@@ -3723,45 +3717,45 @@
       <c r="K55" s="67"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="119"/>
-      <c r="C56" s="120"/>
-      <c r="D56" s="120"/>
-      <c r="E56" s="125"/>
-      <c r="F56" s="129"/>
-      <c r="G56" s="130"/>
-      <c r="H56" s="125"/>
-      <c r="I56" s="125"/>
+      <c r="B56" s="117"/>
+      <c r="C56" s="118"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="123"/>
+      <c r="F56" s="127"/>
+      <c r="G56" s="128"/>
+      <c r="H56" s="123"/>
+      <c r="I56" s="123"/>
       <c r="K56" s="67"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="119">
+      <c r="B57" s="117">
         <v>9</v>
       </c>
-      <c r="C57" s="120">
+      <c r="C57" s="118">
         <v>100</v>
       </c>
-      <c r="D57" s="121" t="s">
+      <c r="D57" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="120"/>
-      <c r="F57" s="121" t="s">
+      <c r="E57" s="118"/>
+      <c r="F57" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="122">
+      <c r="G57" s="120">
         <v>888.8</v>
       </c>
-      <c r="H57" s="125"/>
-      <c r="I57" s="125"/>
-      <c r="J57" s="116"/>
-      <c r="K57" s="123">
+      <c r="H57" s="123"/>
+      <c r="I57" s="123"/>
+      <c r="J57" s="114"/>
+      <c r="K57" s="121">
         <f>IF(COUNTA(J58:J61)&lt;3,0,IF(COUNTA(J58:J61)=3,SUM(J58:J61),IF(SUM(J58:J61)&gt;0,SUM(J58:J61)-MINA(J58:J61),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="119"/>
-      <c r="C58" s="120"/>
-      <c r="D58" s="120"/>
+      <c r="B58" s="117"/>
+      <c r="C58" s="118"/>
+      <c r="D58" s="118"/>
       <c r="E58" s="8">
         <v>123456</v>
       </c>
@@ -3784,9 +3778,9 @@
       <c r="K58" s="67"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B59" s="119"/>
-      <c r="C59" s="120"/>
-      <c r="D59" s="120"/>
+      <c r="B59" s="117"/>
+      <c r="C59" s="118"/>
+      <c r="D59" s="118"/>
       <c r="E59" s="8">
         <v>123456</v>
       </c>
@@ -3809,9 +3803,9 @@
       <c r="K59" s="67"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B60" s="119"/>
-      <c r="C60" s="120"/>
-      <c r="D60" s="120"/>
+      <c r="B60" s="117"/>
+      <c r="C60" s="118"/>
+      <c r="D60" s="118"/>
       <c r="E60" s="8">
         <v>123456</v>
       </c>
@@ -3834,9 +3828,9 @@
       <c r="K60" s="67"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B61" s="119"/>
-      <c r="C61" s="120"/>
-      <c r="D61" s="120"/>
+      <c r="B61" s="117"/>
+      <c r="C61" s="118"/>
+      <c r="D61" s="118"/>
       <c r="E61" s="8">
         <v>123456</v>
       </c>
@@ -3859,46 +3853,46 @@
       <c r="K61" s="67"/>
     </row>
     <row r="62" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B62" s="126"/>
+      <c r="B62" s="124"/>
       <c r="C62" s="82"/>
       <c r="D62" s="82"/>
       <c r="E62" s="82"/>
       <c r="F62" s="82"/>
-      <c r="G62" s="127"/>
-      <c r="H62" s="125"/>
-      <c r="I62" s="125"/>
+      <c r="G62" s="125"/>
+      <c r="H62" s="123"/>
+      <c r="I62" s="123"/>
       <c r="J62" s="82"/>
-      <c r="K62" s="128"/>
+      <c r="K62" s="126"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B63" s="119">
+      <c r="B63" s="117">
         <v>10</v>
       </c>
-      <c r="C63" s="120">
+      <c r="C63" s="118">
         <v>100</v>
       </c>
-      <c r="D63" s="121" t="s">
+      <c r="D63" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="120"/>
-      <c r="F63" s="121" t="s">
+      <c r="E63" s="118"/>
+      <c r="F63" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="G63" s="122">
+      <c r="G63" s="120">
         <v>888.8</v>
       </c>
-      <c r="H63" s="125"/>
-      <c r="I63" s="125"/>
-      <c r="J63" s="116"/>
-      <c r="K63" s="123">
+      <c r="H63" s="123"/>
+      <c r="I63" s="123"/>
+      <c r="J63" s="114"/>
+      <c r="K63" s="121">
         <f>IF(COUNTA(J64:J67)&lt;3,0,IF(COUNTA(J64:J67)=3,SUM(J64:J67),IF(SUM(J64:J67)&gt;0,SUM(J64:J67)-MINA(J64:J67),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B64" s="119"/>
-      <c r="C64" s="120"/>
-      <c r="D64" s="120"/>
+      <c r="B64" s="117"/>
+      <c r="C64" s="118"/>
+      <c r="D64" s="118"/>
       <c r="E64" s="8">
         <v>123456</v>
       </c>
@@ -3921,9 +3915,9 @@
       <c r="K64" s="67"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="119"/>
-      <c r="C65" s="120"/>
-      <c r="D65" s="120"/>
+      <c r="B65" s="117"/>
+      <c r="C65" s="118"/>
+      <c r="D65" s="118"/>
       <c r="E65" s="8">
         <v>123456</v>
       </c>
@@ -3946,9 +3940,9 @@
       <c r="K65" s="67"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B66" s="119"/>
-      <c r="C66" s="120"/>
-      <c r="D66" s="120"/>
+      <c r="B66" s="117"/>
+      <c r="C66" s="118"/>
+      <c r="D66" s="118"/>
       <c r="E66" s="8">
         <v>123456</v>
       </c>
@@ -3971,9 +3965,9 @@
       <c r="K66" s="67"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B67" s="119"/>
-      <c r="C67" s="120"/>
-      <c r="D67" s="120"/>
+      <c r="B67" s="117"/>
+      <c r="C67" s="118"/>
+      <c r="D67" s="118"/>
       <c r="E67" s="8">
         <v>123456</v>
       </c>
@@ -3996,40 +3990,40 @@
       <c r="K67" s="67"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B68" s="115"/>
-      <c r="H68" s="125"/>
-      <c r="I68" s="125"/>
+      <c r="B68" s="113"/>
+      <c r="H68" s="123"/>
+      <c r="I68" s="123"/>
       <c r="K68" s="67"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B69" s="119">
+      <c r="B69" s="117">
         <v>11</v>
       </c>
-      <c r="C69" s="120">
+      <c r="C69" s="118">
         <v>100</v>
       </c>
-      <c r="D69" s="121" t="s">
+      <c r="D69" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="E69" s="120"/>
-      <c r="F69" s="121" t="s">
+      <c r="E69" s="118"/>
+      <c r="F69" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="G69" s="122">
+      <c r="G69" s="120">
         <v>888.8</v>
       </c>
-      <c r="H69" s="125"/>
-      <c r="I69" s="125"/>
-      <c r="J69" s="116"/>
-      <c r="K69" s="123">
+      <c r="H69" s="123"/>
+      <c r="I69" s="123"/>
+      <c r="J69" s="114"/>
+      <c r="K69" s="121">
         <f>IF(COUNTA(J70:J73)&lt;3,0,IF(COUNTA(J70:J73)=3,SUM(J70:J73),IF(SUM(J70:J73)&gt;0,SUM(J70:J73)-MINA(J70:J73),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B70" s="119"/>
-      <c r="C70" s="120"/>
-      <c r="D70" s="120"/>
+      <c r="B70" s="117"/>
+      <c r="C70" s="118"/>
+      <c r="D70" s="118"/>
       <c r="E70" s="8">
         <v>123456</v>
       </c>
@@ -4052,9 +4046,9 @@
       <c r="K70" s="67"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="119"/>
-      <c r="C71" s="120"/>
-      <c r="D71" s="120"/>
+      <c r="B71" s="117"/>
+      <c r="C71" s="118"/>
+      <c r="D71" s="118"/>
       <c r="E71" s="8">
         <v>123456</v>
       </c>
@@ -4077,9 +4071,9 @@
       <c r="K71" s="67"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B72" s="119"/>
-      <c r="C72" s="120"/>
-      <c r="D72" s="120"/>
+      <c r="B72" s="117"/>
+      <c r="C72" s="118"/>
+      <c r="D72" s="118"/>
       <c r="E72" s="8">
         <v>123456</v>
       </c>
@@ -4102,9 +4096,9 @@
       <c r="K72" s="67"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B73" s="119"/>
-      <c r="C73" s="120"/>
-      <c r="D73" s="120"/>
+      <c r="B73" s="117"/>
+      <c r="C73" s="118"/>
+      <c r="D73" s="118"/>
       <c r="E73" s="8">
         <v>123456</v>
       </c>
@@ -4127,40 +4121,40 @@
       <c r="K73" s="67"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B74" s="115"/>
-      <c r="H74" s="125"/>
-      <c r="I74" s="125"/>
+      <c r="B74" s="113"/>
+      <c r="H74" s="123"/>
+      <c r="I74" s="123"/>
       <c r="K74" s="67"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B75" s="119">
+      <c r="B75" s="117">
         <v>12</v>
       </c>
-      <c r="C75" s="120">
+      <c r="C75" s="118">
         <v>100</v>
       </c>
-      <c r="D75" s="121" t="s">
+      <c r="D75" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="120"/>
-      <c r="F75" s="121" t="s">
+      <c r="E75" s="118"/>
+      <c r="F75" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="G75" s="122">
+      <c r="G75" s="120">
         <v>888.8</v>
       </c>
-      <c r="H75" s="125"/>
-      <c r="I75" s="125"/>
-      <c r="J75" s="116"/>
-      <c r="K75" s="123">
+      <c r="H75" s="123"/>
+      <c r="I75" s="123"/>
+      <c r="J75" s="114"/>
+      <c r="K75" s="121">
         <f>IF(COUNTA(J76:J79)&lt;3,0,IF(COUNTA(J76:J79)=3,SUM(J76:J79),IF(SUM(J76:J79)&gt;0,SUM(J76:J79)-MINA(J76:J79),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="119"/>
-      <c r="C76" s="120"/>
-      <c r="D76" s="120"/>
+      <c r="B76" s="117"/>
+      <c r="C76" s="118"/>
+      <c r="D76" s="118"/>
       <c r="E76" s="8">
         <v>123456</v>
       </c>
@@ -4183,9 +4177,9 @@
       <c r="K76" s="67"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="119"/>
-      <c r="C77" s="120"/>
-      <c r="D77" s="120"/>
+      <c r="B77" s="117"/>
+      <c r="C77" s="118"/>
+      <c r="D77" s="118"/>
       <c r="E77" s="8">
         <v>123456</v>
       </c>
@@ -4208,9 +4202,9 @@
       <c r="K77" s="67"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B78" s="119"/>
-      <c r="C78" s="120"/>
-      <c r="D78" s="120"/>
+      <c r="B78" s="117"/>
+      <c r="C78" s="118"/>
+      <c r="D78" s="118"/>
       <c r="E78" s="8">
         <v>123456</v>
       </c>
@@ -4233,9 +4227,9 @@
       <c r="K78" s="67"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B79" s="119"/>
-      <c r="C79" s="120"/>
-      <c r="D79" s="120"/>
+      <c r="B79" s="117"/>
+      <c r="C79" s="118"/>
+      <c r="D79" s="118"/>
       <c r="E79" s="8">
         <v>123456</v>
       </c>
@@ -4258,20 +4252,20 @@
       <c r="K79" s="67"/>
     </row>
     <row r="80" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="133"/>
-      <c r="C80" s="134"/>
-      <c r="D80" s="134"/>
-      <c r="E80" s="135"/>
-      <c r="F80" s="135"/>
-      <c r="G80" s="136"/>
-      <c r="H80" s="131"/>
-      <c r="I80" s="131"/>
-      <c r="J80" s="131"/>
-      <c r="K80" s="132"/>
+      <c r="B80" s="131"/>
+      <c r="C80" s="132"/>
+      <c r="D80" s="132"/>
+      <c r="E80" s="133"/>
+      <c r="F80" s="133"/>
+      <c r="G80" s="134"/>
+      <c r="H80" s="129"/>
+      <c r="I80" s="129"/>
+      <c r="J80" s="129"/>
+      <c r="K80" s="130"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2"/>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="124" t="s">
+      <c r="B82" s="122" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4358,31 +4352,31 @@
     </row>
     <row r="2" spans="1:28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="82"/>
-      <c r="B2" s="153" t="str">
+      <c r="B2" s="151" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>RK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="154"/>
-      <c r="S2" s="154"/>
-      <c r="T2" s="154"/>
-      <c r="U2" s="154"/>
-      <c r="V2" s="154"/>
-      <c r="W2" s="155"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
+      <c r="Q2" s="152"/>
+      <c r="R2" s="152"/>
+      <c r="S2" s="152"/>
+      <c r="T2" s="152"/>
+      <c r="U2" s="152"/>
+      <c r="V2" s="152"/>
+      <c r="W2" s="153"/>
       <c r="X2" s="82"/>
       <c r="Y2" s="82"/>
       <c r="Z2" s="82"/>
@@ -4420,7 +4414,7 @@
       <c r="B4" s="82"/>
       <c r="C4" s="82"/>
       <c r="D4" s="82"/>
-      <c r="E4" s="93"/>
+      <c r="E4" s="91"/>
       <c r="F4" s="82"/>
       <c r="G4" s="82"/>
       <c r="H4" s="82"/>
@@ -4430,20 +4424,20 @@
       <c r="L4" s="82"/>
       <c r="M4" s="82"/>
       <c r="N4" s="82"/>
-      <c r="O4" s="94" t="s">
+      <c r="O4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="156" t="str">
+      <c r="P4" s="154" t="str">
         <f>'Deelnemers en Scores'!H4</f>
         <v>yyyy-mm-dd</v>
       </c>
-      <c r="Q4" s="157"/>
-      <c r="R4" s="157"/>
-      <c r="S4" s="157"/>
-      <c r="T4" s="157"/>
-      <c r="U4" s="157"/>
-      <c r="V4" s="95"/>
-      <c r="W4" s="96"/>
+      <c r="Q4" s="155"/>
+      <c r="R4" s="155"/>
+      <c r="S4" s="155"/>
+      <c r="T4" s="155"/>
+      <c r="U4" s="155"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="94"/>
       <c r="X4" s="82"/>
       <c r="Y4" s="82"/>
       <c r="Z4" s="82"/>
@@ -4506,38 +4500,38 @@
     </row>
     <row r="7" spans="1:28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="82"/>
-      <c r="B7" s="97"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="151" t="s">
+      <c r="B7" s="95"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="158" t="s">
+      <c r="F7" s="156"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="156"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="158"/>
-      <c r="L7" s="158"/>
-      <c r="M7" s="152"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="151" t="s">
+      <c r="K7" s="156"/>
+      <c r="L7" s="156"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="158"/>
-      <c r="R7" s="152"/>
-      <c r="S7" s="100" t="s">
+      <c r="P7" s="156"/>
+      <c r="Q7" s="156"/>
+      <c r="R7" s="150"/>
+      <c r="S7" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="T7" s="151" t="s">
+      <c r="T7" s="149" t="s">
         <v>86</v>
       </c>
-      <c r="U7" s="152"/>
-      <c r="V7" s="101"/>
-      <c r="W7" s="102" t="s">
+      <c r="U7" s="150"/>
+      <c r="V7" s="99"/>
+      <c r="W7" s="100" t="s">
         <v>85</v>
       </c>
       <c r="X7" s="82"/>
@@ -4546,64 +4540,64 @@
     </row>
     <row r="8" spans="1:28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="83"/>
-      <c r="B8" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="104" t="s">
+      <c r="B8" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="104" t="s">
+      <c r="D8" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="105">
+      <c r="E8" s="103">
         <v>1</v>
       </c>
-      <c r="F8" s="106">
+      <c r="F8" s="104">
         <v>2</v>
       </c>
-      <c r="G8" s="106">
+      <c r="G8" s="104">
         <v>3</v>
       </c>
-      <c r="H8" s="107">
+      <c r="H8" s="105">
         <v>4</v>
       </c>
-      <c r="I8" s="108"/>
-      <c r="J8" s="105">
+      <c r="I8" s="106"/>
+      <c r="J8" s="103">
         <v>1</v>
       </c>
-      <c r="K8" s="106">
+      <c r="K8" s="104">
         <v>2</v>
       </c>
-      <c r="L8" s="106">
+      <c r="L8" s="104">
         <v>3</v>
       </c>
-      <c r="M8" s="109">
+      <c r="M8" s="107">
         <v>4</v>
       </c>
-      <c r="N8" s="108"/>
-      <c r="O8" s="105">
+      <c r="N8" s="106"/>
+      <c r="O8" s="103">
         <v>1</v>
       </c>
-      <c r="P8" s="106">
+      <c r="P8" s="104">
         <v>2</v>
       </c>
-      <c r="Q8" s="106">
+      <c r="Q8" s="104">
         <v>3</v>
       </c>
-      <c r="R8" s="109">
+      <c r="R8" s="107">
         <v>4</v>
       </c>
-      <c r="S8" s="110" t="s">
+      <c r="S8" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="T8" s="111" t="s">
+      <c r="T8" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="112" t="s">
+      <c r="U8" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="V8" s="108"/>
-      <c r="W8" s="110"/>
+      <c r="V8" s="106"/>
+      <c r="W8" s="108"/>
       <c r="X8" s="82"/>
       <c r="Y8" s="82"/>
       <c r="Z8" s="82"/>
@@ -4657,44 +4651,44 @@
       </c>
       <c r="N9" s="88"/>
       <c r="O9" s="56" t="str">
-        <f t="shared" ref="O9:O20" si="0">IF(ISNUMBER(J9),E9+J9,"")</f>
+        <f>IF(ISNUMBER(J9),E9+J9,"")</f>
         <v/>
       </c>
       <c r="P9" s="57" t="str">
-        <f t="shared" ref="P9:P20" si="1">IF(ISNUMBER(K9),F9+K9,"")</f>
+        <f>IF(ISNUMBER(K9),F9+K9,"")</f>
         <v/>
       </c>
       <c r="Q9" s="57" t="str">
-        <f t="shared" ref="Q9:Q20" si="2">IF(ISNUMBER(L9),G9+L9,"")</f>
+        <f>IF(ISNUMBER(L9),G9+L9,"")</f>
         <v/>
       </c>
       <c r="R9" s="58" t="str">
-        <f t="shared" ref="R9:R20" si="3">IF(ISNUMBER(M9),H9+M9,"")</f>
+        <f>IF(ISNUMBER(M9),H9+M9,"")</f>
         <v/>
       </c>
       <c r="S9" s="60">
-        <f t="shared" ref="S9:S20" si="4">IF(COUNT(O9:R9)&lt;4,SUM(O9:R9),SUM(O9:R9)-MIN(O9:R9))</f>
+        <f>IF(COUNT(O9:R9)&lt;4,SUM(O9:R9),SUM(O9:R9)-MIN(O9:R9))</f>
         <v>0</v>
       </c>
       <c r="T9" s="56">
-        <f t="shared" ref="T9:T20" si="5">LARGE(O9:R9,1)</f>
+        <f>IF(S9&gt;0,LARGE(O9:R9,1),0)</f>
         <v>0</v>
       </c>
       <c r="U9" s="58">
-        <f t="shared" ref="U9:U20" si="6">LARGE(O9:R9,2)</f>
+        <f>IF(S9&gt;0,LARGE(O9:R9,2),0)</f>
         <v>0</v>
       </c>
       <c r="V9" s="88"/>
       <c r="W9" s="59">
-        <f>S9+D23</f>
+        <f>S9+T9/10000+U9/10000000</f>
         <v>0</v>
       </c>
       <c r="X9" s="86"/>
-      <c r="Y9" s="113" t="str">
+      <c r="Y9" s="111" t="str">
         <f>IF(W9&gt;0,IF(W9=W8,Y8,ROW()-ROW($Y$8)),"")</f>
         <v/>
       </c>
-      <c r="Z9" s="114" t="str">
+      <c r="Z9" s="112" t="str">
         <f>IF(Y9&lt;&gt;"","e","")</f>
         <v/>
       </c>
@@ -4704,273 +4698,273 @@
     <row r="10" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="83"/>
       <c r="B10" s="49">
-        <f>IF('Deelnemers en Scores'!B27&gt;0,'Deelnemers en Scores'!B27,"")</f>
-        <v>4</v>
+        <f>IF('Deelnemers en Scores'!B15&gt;0,'Deelnemers en Scores'!B15,"")</f>
+        <v>2</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f>IF('Deelnemers en Scores'!F27="","",'Deelnemers en Scores'!F27)</f>
-        <v>Team naam 4</v>
+        <f>IF('Deelnemers en Scores'!F15="","",'Deelnemers en Scores'!F15)</f>
+        <v>Team naam 2</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f>'Deelnemers en Scores'!D27</f>
-        <v>Vereniging 4</v>
+        <f>'Deelnemers en Scores'!D15</f>
+        <v>Vereniging 2</v>
       </c>
       <c r="E10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H28=0,"",'Deelnemers en Scores'!H28)</f>
+        <f>IF('Deelnemers en Scores'!H16=0,"",'Deelnemers en Scores'!H16)</f>
         <v/>
       </c>
       <c r="F10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H29=0,"",'Deelnemers en Scores'!H29)</f>
+        <f>IF('Deelnemers en Scores'!H17=0,"",'Deelnemers en Scores'!H17)</f>
         <v/>
       </c>
       <c r="G10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H30=0,"",'Deelnemers en Scores'!H30)</f>
+        <f>IF('Deelnemers en Scores'!H18=0,"",'Deelnemers en Scores'!H18)</f>
         <v/>
       </c>
       <c r="H10" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!H31=0,"",'Deelnemers en Scores'!H31)</f>
+        <f>IF('Deelnemers en Scores'!H19=0,"",'Deelnemers en Scores'!H19)</f>
         <v/>
       </c>
       <c r="I10" s="89"/>
       <c r="J10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I28=0,"",'Deelnemers en Scores'!I28)</f>
+        <f>IF('Deelnemers en Scores'!I16=0,"",'Deelnemers en Scores'!I16)</f>
         <v/>
       </c>
       <c r="K10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I29=0,"",'Deelnemers en Scores'!I29)</f>
+        <f>IF('Deelnemers en Scores'!I17=0,"",'Deelnemers en Scores'!I17)</f>
         <v/>
       </c>
       <c r="L10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I30=0,"",'Deelnemers en Scores'!I30)</f>
+        <f>IF('Deelnemers en Scores'!I18=0,"",'Deelnemers en Scores'!I18)</f>
         <v/>
       </c>
       <c r="M10" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!I31=0,"",'Deelnemers en Scores'!I31)</f>
+        <f>IF('Deelnemers en Scores'!I19=0,"",'Deelnemers en Scores'!I19)</f>
         <v/>
       </c>
       <c r="N10" s="89"/>
       <c r="O10" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J10),E10+J10,"")</f>
         <v/>
       </c>
       <c r="P10" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K10),F10+K10,"")</f>
         <v/>
       </c>
       <c r="Q10" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L10),G10+L10,"")</f>
         <v/>
       </c>
       <c r="R10" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M10),H10+M10,"")</f>
         <v/>
       </c>
       <c r="S10" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O10:R10)&lt;4,SUM(O10:R10),SUM(O10:R10)-MIN(O10:R10))</f>
         <v>0</v>
       </c>
       <c r="T10" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S10&gt;0,LARGE(O10:R10,1),0)</f>
         <v>0</v>
       </c>
       <c r="U10" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S10&gt;0,LARGE(O10:R10,2),0)</f>
         <v>0</v>
       </c>
       <c r="V10" s="89"/>
       <c r="W10" s="59">
-        <f t="shared" ref="W10:W20" si="7">S10+T10/10000+U10/10000000</f>
+        <f>S10+T10/10000+U10/10000000</f>
         <v>0</v>
       </c>
       <c r="X10" s="86"/>
-      <c r="Y10" s="113" t="str">
-        <f t="shared" ref="Y10:Y20" si="8">IF(W10&gt;0,IF(W10=W9,Y9,ROW()-ROW($Y$8)),"")</f>
-        <v/>
-      </c>
-      <c r="Z10" s="114" t="str">
-        <f t="shared" ref="Z10:Z20" si="9">IF(Y10&lt;&gt;"","e","")</f>
+      <c r="Y10" s="111" t="str">
+        <f t="shared" ref="Y10:Y20" si="0">IF(W10&gt;0,IF(W10=W9,Y9,ROW()-ROW($Y$8)),"")</f>
+        <v/>
+      </c>
+      <c r="Z10" s="112" t="str">
+        <f t="shared" ref="Z10:Z20" si="1">IF(Y10&lt;&gt;"","e","")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="83"/>
       <c r="B11" s="49">
-        <f>IF('Deelnemers en Scores'!B15&gt;0,'Deelnemers en Scores'!B15,"")</f>
-        <v>2</v>
+        <f>IF('Deelnemers en Scores'!B21&gt;0,'Deelnemers en Scores'!B21,"")</f>
+        <v>3</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>IF('Deelnemers en Scores'!F15="","",'Deelnemers en Scores'!F15)</f>
-        <v>Team naam 2</v>
+        <f>IF('Deelnemers en Scores'!F21="","",'Deelnemers en Scores'!F21)</f>
+        <v>Team naam 3</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f>'Deelnemers en Scores'!D15</f>
-        <v>Vereniging 2</v>
+        <f>'Deelnemers en Scores'!D21</f>
+        <v>Vereniging 3</v>
       </c>
       <c r="E11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H16=0,"",'Deelnemers en Scores'!H16)</f>
+        <f>IF('Deelnemers en Scores'!H22=0,"",'Deelnemers en Scores'!H22)</f>
         <v/>
       </c>
       <c r="F11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H17=0,"",'Deelnemers en Scores'!H17)</f>
+        <f>IF('Deelnemers en Scores'!H23=0,"",'Deelnemers en Scores'!H23)</f>
         <v/>
       </c>
       <c r="G11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H18=0,"",'Deelnemers en Scores'!H18)</f>
+        <f>IF('Deelnemers en Scores'!H24=0,"",'Deelnemers en Scores'!H24)</f>
         <v/>
       </c>
       <c r="H11" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!H19=0,"",'Deelnemers en Scores'!H19)</f>
+        <f>IF('Deelnemers en Scores'!H25=0,"",'Deelnemers en Scores'!H25)</f>
         <v/>
       </c>
       <c r="I11" s="89"/>
       <c r="J11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I16=0,"",'Deelnemers en Scores'!I16)</f>
+        <f>IF('Deelnemers en Scores'!I22=0,"",'Deelnemers en Scores'!I22)</f>
         <v/>
       </c>
       <c r="K11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I17=0,"",'Deelnemers en Scores'!I17)</f>
+        <f>IF('Deelnemers en Scores'!I23=0,"",'Deelnemers en Scores'!I23)</f>
         <v/>
       </c>
       <c r="L11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I18=0,"",'Deelnemers en Scores'!I18)</f>
+        <f>IF('Deelnemers en Scores'!I24=0,"",'Deelnemers en Scores'!I24)</f>
         <v/>
       </c>
       <c r="M11" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!I19=0,"",'Deelnemers en Scores'!I19)</f>
+        <f>IF('Deelnemers en Scores'!I25=0,"",'Deelnemers en Scores'!I25)</f>
         <v/>
       </c>
       <c r="N11" s="89"/>
       <c r="O11" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J11),E11+J11,"")</f>
         <v/>
       </c>
       <c r="P11" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K11),F11+K11,"")</f>
         <v/>
       </c>
       <c r="Q11" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L11),G11+L11,"")</f>
         <v/>
       </c>
       <c r="R11" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M11),H11+M11,"")</f>
         <v/>
       </c>
       <c r="S11" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O11:R11)&lt;4,SUM(O11:R11),SUM(O11:R11)-MIN(O11:R11))</f>
         <v>0</v>
       </c>
       <c r="T11" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S11&gt;0,LARGE(O11:R11,1),0)</f>
         <v>0</v>
       </c>
       <c r="U11" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S11&gt;0,LARGE(O11:R11,2),0)</f>
         <v>0</v>
       </c>
       <c r="V11" s="89"/>
       <c r="W11" s="59">
-        <f t="shared" si="7"/>
+        <f>S11+T11/10000+U11/10000000</f>
         <v>0</v>
       </c>
       <c r="X11" s="86"/>
-      <c r="Y11" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z11" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y11" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z11" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="83"/>
       <c r="B12" s="49">
-        <f>IF('Deelnemers en Scores'!B21&gt;0,'Deelnemers en Scores'!B21,"")</f>
-        <v>3</v>
+        <f>IF('Deelnemers en Scores'!B27&gt;0,'Deelnemers en Scores'!B27,"")</f>
+        <v>4</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>IF('Deelnemers en Scores'!F21="","",'Deelnemers en Scores'!F21)</f>
-        <v>Team naam 3</v>
+        <f>IF('Deelnemers en Scores'!F27="","",'Deelnemers en Scores'!F27)</f>
+        <v>Team naam 4</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f>'Deelnemers en Scores'!D21</f>
-        <v>Vereniging 3</v>
+        <f>'Deelnemers en Scores'!D27</f>
+        <v>Vereniging 4</v>
       </c>
       <c r="E12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H22=0,"",'Deelnemers en Scores'!H22)</f>
+        <f>IF('Deelnemers en Scores'!H28=0,"",'Deelnemers en Scores'!H28)</f>
         <v/>
       </c>
       <c r="F12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H23=0,"",'Deelnemers en Scores'!H23)</f>
+        <f>IF('Deelnemers en Scores'!H29=0,"",'Deelnemers en Scores'!H29)</f>
         <v/>
       </c>
       <c r="G12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H24=0,"",'Deelnemers en Scores'!H24)</f>
+        <f>IF('Deelnemers en Scores'!H30=0,"",'Deelnemers en Scores'!H30)</f>
         <v/>
       </c>
       <c r="H12" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!H25=0,"",'Deelnemers en Scores'!H25)</f>
+        <f>IF('Deelnemers en Scores'!H31=0,"",'Deelnemers en Scores'!H31)</f>
         <v/>
       </c>
       <c r="I12" s="89"/>
       <c r="J12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I22=0,"",'Deelnemers en Scores'!I22)</f>
+        <f>IF('Deelnemers en Scores'!I28=0,"",'Deelnemers en Scores'!I28)</f>
         <v/>
       </c>
       <c r="K12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I23=0,"",'Deelnemers en Scores'!I23)</f>
+        <f>IF('Deelnemers en Scores'!I29=0,"",'Deelnemers en Scores'!I29)</f>
         <v/>
       </c>
       <c r="L12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I24=0,"",'Deelnemers en Scores'!I24)</f>
+        <f>IF('Deelnemers en Scores'!I30=0,"",'Deelnemers en Scores'!I30)</f>
         <v/>
       </c>
       <c r="M12" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!I25=0,"",'Deelnemers en Scores'!I25)</f>
+        <f>IF('Deelnemers en Scores'!I31=0,"",'Deelnemers en Scores'!I31)</f>
         <v/>
       </c>
       <c r="N12" s="89"/>
       <c r="O12" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J12),E12+J12,"")</f>
         <v/>
       </c>
       <c r="P12" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K12),F12+K12,"")</f>
         <v/>
       </c>
       <c r="Q12" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L12),G12+L12,"")</f>
         <v/>
       </c>
       <c r="R12" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M12),H12+M12,"")</f>
         <v/>
       </c>
       <c r="S12" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O12:R12)&lt;4,SUM(O12:R12),SUM(O12:R12)-MIN(O12:R12))</f>
         <v>0</v>
       </c>
       <c r="T12" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S12&gt;0,LARGE(O12:R12,1),0)</f>
         <v>0</v>
       </c>
       <c r="U12" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S12&gt;0,LARGE(O12:R12,2),0)</f>
         <v>0</v>
       </c>
       <c r="V12" s="89"/>
       <c r="W12" s="59">
-        <f t="shared" si="7"/>
+        <f>S12+T12/10000+U12/10000000</f>
         <v>0</v>
       </c>
       <c r="X12" s="86"/>
-      <c r="Y12" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z12" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y12" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z12" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5023,45 +5017,45 @@
       </c>
       <c r="N13" s="89"/>
       <c r="O13" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J13),E13+J13,"")</f>
         <v/>
       </c>
       <c r="P13" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K13),F13+K13,"")</f>
         <v/>
       </c>
       <c r="Q13" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L13),G13+L13,"")</f>
         <v/>
       </c>
       <c r="R13" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M13),H13+M13,"")</f>
         <v/>
       </c>
       <c r="S13" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O13:R13)&lt;4,SUM(O13:R13),SUM(O13:R13)-MIN(O13:R13))</f>
         <v>0</v>
       </c>
       <c r="T13" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S13&gt;0,LARGE(O13:R13,1),0)</f>
         <v>0</v>
       </c>
       <c r="U13" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S13&gt;0,LARGE(O13:R13,2),0)</f>
         <v>0</v>
       </c>
       <c r="V13" s="89"/>
       <c r="W13" s="59">
-        <f t="shared" si="7"/>
+        <f>S13+T13/10000+U13/10000000</f>
         <v>0</v>
       </c>
       <c r="X13" s="86"/>
-      <c r="Y13" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z13" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y13" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z13" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5114,45 +5108,45 @@
       </c>
       <c r="N14" s="89"/>
       <c r="O14" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J14),E14+J14,"")</f>
         <v/>
       </c>
       <c r="P14" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K14),F14+K14,"")</f>
         <v/>
       </c>
       <c r="Q14" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L14),G14+L14,"")</f>
         <v/>
       </c>
       <c r="R14" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M14),H14+M14,"")</f>
         <v/>
       </c>
       <c r="S14" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O14:R14)&lt;4,SUM(O14:R14),SUM(O14:R14)-MIN(O14:R14))</f>
         <v>0</v>
       </c>
       <c r="T14" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S14&gt;0,LARGE(O14:R14,1),0)</f>
         <v>0</v>
       </c>
       <c r="U14" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S14&gt;0,LARGE(O14:R14,2),0)</f>
         <v>0</v>
       </c>
       <c r="V14" s="89"/>
       <c r="W14" s="59">
-        <f t="shared" si="7"/>
+        <f>S14+T14/10000+U14/10000000</f>
         <v>0</v>
       </c>
       <c r="X14" s="86"/>
-      <c r="Y14" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z14" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y14" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z14" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5205,45 +5199,45 @@
       </c>
       <c r="N15" s="89"/>
       <c r="O15" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J15),E15+J15,"")</f>
         <v/>
       </c>
       <c r="P15" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K15),F15+K15,"")</f>
         <v/>
       </c>
       <c r="Q15" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L15),G15+L15,"")</f>
         <v/>
       </c>
       <c r="R15" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M15),H15+M15,"")</f>
         <v/>
       </c>
       <c r="S15" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O15:R15)&lt;4,SUM(O15:R15),SUM(O15:R15)-MIN(O15:R15))</f>
         <v>0</v>
       </c>
       <c r="T15" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S15&gt;0,LARGE(O15:R15,1),0)</f>
         <v>0</v>
       </c>
       <c r="U15" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S15&gt;0,LARGE(O15:R15,2),0)</f>
         <v>0</v>
       </c>
       <c r="V15" s="89"/>
       <c r="W15" s="59">
-        <f t="shared" si="7"/>
+        <f>S15+T15/10000+U15/10000000</f>
         <v>0</v>
       </c>
       <c r="X15" s="86"/>
-      <c r="Y15" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z15" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y15" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z15" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5296,45 +5290,45 @@
       </c>
       <c r="N16" s="89"/>
       <c r="O16" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J16),E16+J16,"")</f>
         <v/>
       </c>
       <c r="P16" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K16),F16+K16,"")</f>
         <v/>
       </c>
       <c r="Q16" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L16),G16+L16,"")</f>
         <v/>
       </c>
       <c r="R16" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M16),H16+M16,"")</f>
         <v/>
       </c>
       <c r="S16" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O16:R16)&lt;4,SUM(O16:R16),SUM(O16:R16)-MIN(O16:R16))</f>
         <v>0</v>
       </c>
       <c r="T16" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S16&gt;0,LARGE(O16:R16,1),0)</f>
         <v>0</v>
       </c>
       <c r="U16" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S16&gt;0,LARGE(O16:R16,2),0)</f>
         <v>0</v>
       </c>
       <c r="V16" s="89"/>
       <c r="W16" s="59">
-        <f t="shared" si="7"/>
+        <f>S16+T16/10000+U16/10000000</f>
         <v>0</v>
       </c>
       <c r="X16" s="86"/>
-      <c r="Y16" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z16" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y16" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z16" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5387,45 +5381,45 @@
       </c>
       <c r="N17" s="89"/>
       <c r="O17" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J17),E17+J17,"")</f>
         <v/>
       </c>
       <c r="P17" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K17),F17+K17,"")</f>
         <v/>
       </c>
       <c r="Q17" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L17),G17+L17,"")</f>
         <v/>
       </c>
       <c r="R17" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M17),H17+M17,"")</f>
         <v/>
       </c>
       <c r="S17" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O17:R17)&lt;4,SUM(O17:R17),SUM(O17:R17)-MIN(O17:R17))</f>
         <v>0</v>
       </c>
       <c r="T17" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S17&gt;0,LARGE(O17:R17,1),0)</f>
         <v>0</v>
       </c>
       <c r="U17" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S17&gt;0,LARGE(O17:R17,2),0)</f>
         <v>0</v>
       </c>
       <c r="V17" s="89"/>
       <c r="W17" s="59">
-        <f t="shared" si="7"/>
+        <f>S17+T17/10000+U17/10000000</f>
         <v>0</v>
       </c>
       <c r="X17" s="86"/>
-      <c r="Y17" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z17" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y17" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z17" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5478,45 +5472,45 @@
       </c>
       <c r="N18" s="89"/>
       <c r="O18" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J18),E18+J18,"")</f>
         <v/>
       </c>
       <c r="P18" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K18),F18+K18,"")</f>
         <v/>
       </c>
       <c r="Q18" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L18),G18+L18,"")</f>
         <v/>
       </c>
       <c r="R18" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M18),H18+M18,"")</f>
         <v/>
       </c>
       <c r="S18" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O18:R18)&lt;4,SUM(O18:R18),SUM(O18:R18)-MIN(O18:R18))</f>
         <v>0</v>
       </c>
       <c r="T18" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S18&gt;0,LARGE(O18:R18,1),0)</f>
         <v>0</v>
       </c>
       <c r="U18" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S18&gt;0,LARGE(O18:R18,2),0)</f>
         <v>0</v>
       </c>
       <c r="V18" s="89"/>
       <c r="W18" s="59">
-        <f t="shared" si="7"/>
+        <f>S18+T18/10000+U18/10000000</f>
         <v>0</v>
       </c>
       <c r="X18" s="86"/>
-      <c r="Y18" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z18" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y18" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z18" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5569,45 +5563,45 @@
       </c>
       <c r="N19" s="89"/>
       <c r="O19" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J19),E19+J19,"")</f>
         <v/>
       </c>
       <c r="P19" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K19),F19+K19,"")</f>
         <v/>
       </c>
       <c r="Q19" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L19),G19+L19,"")</f>
         <v/>
       </c>
       <c r="R19" s="21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M19),H19+M19,"")</f>
         <v/>
       </c>
       <c r="S19" s="60">
-        <f t="shared" si="4"/>
+        <f>IF(COUNT(O19:R19)&lt;4,SUM(O19:R19),SUM(O19:R19)-MIN(O19:R19))</f>
         <v>0</v>
       </c>
       <c r="T19" s="56">
-        <f t="shared" si="5"/>
+        <f>IF(S19&gt;0,LARGE(O19:R19,1),0)</f>
         <v>0</v>
       </c>
       <c r="U19" s="58">
-        <f t="shared" si="6"/>
+        <f>IF(S19&gt;0,LARGE(O19:R19,2),0)</f>
         <v>0</v>
       </c>
       <c r="V19" s="89"/>
       <c r="W19" s="59">
-        <f t="shared" si="7"/>
+        <f>S19+T19/10000+U19/10000000</f>
         <v>0</v>
       </c>
       <c r="X19" s="86"/>
-      <c r="Y19" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z19" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y19" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z19" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5660,45 +5654,45 @@
       </c>
       <c r="N20" s="90"/>
       <c r="O20" s="46" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(J20),E20+J20,"")</f>
         <v/>
       </c>
       <c r="P20" s="47" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(K20),F20+K20,"")</f>
         <v/>
       </c>
       <c r="Q20" s="47" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(L20),G20+L20,"")</f>
         <v/>
       </c>
       <c r="R20" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(M20),H20+M20,"")</f>
         <v/>
       </c>
       <c r="S20" s="60">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="91">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U20" s="92">
-        <f t="shared" si="6"/>
+        <f>IF(COUNT(O20:R20)&lt;4,SUM(O20:R20),SUM(O20:R20)-MIN(O20:R20))</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="56">
+        <f>IF(S20&gt;0,LARGE(O20:R20,1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="58">
+        <f>IF(S20&gt;0,LARGE(O20:R20,2),0)</f>
         <v>0</v>
       </c>
       <c r="V20" s="90"/>
       <c r="W20" s="59">
-        <f t="shared" si="7"/>
+        <f>S20+T20/10000+U20/10000000</f>
         <v>0</v>
       </c>
       <c r="X20" s="86"/>
-      <c r="Y20" s="113" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z20" s="114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Y20" s="111" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z20" s="112" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5731,21 +5725,21 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K23" s="150" t="s">
+      <c r="K23" s="148" t="s">
         <v>84</v>
       </c>
-      <c r="L23" s="150"/>
-      <c r="M23" s="150"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="150"/>
-      <c r="P23" s="150"/>
-      <c r="Q23" s="150"/>
-      <c r="R23" s="150"/>
-      <c r="S23" s="150"/>
-      <c r="T23" s="150"/>
-      <c r="U23" s="150"/>
-      <c r="V23" s="150"/>
-      <c r="W23" s="150"/>
+      <c r="L23" s="148"/>
+      <c r="M23" s="148"/>
+      <c r="N23" s="148"/>
+      <c r="O23" s="148"/>
+      <c r="P23" s="148"/>
+      <c r="Q23" s="148"/>
+      <c r="R23" s="148"/>
+      <c r="S23" s="148"/>
+      <c r="T23" s="148"/>
+      <c r="U23" s="148"/>
+      <c r="V23" s="148"/>
+      <c r="W23" s="148"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="K24" s="87"/>
@@ -5765,7 +5759,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:W20">
-    <sortCondition descending="1" ref="W9"/>
+    <sortCondition ref="B9:B20"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="K23:W23"/>

</xml_diff>